<commit_message>
Modify Temp config to make sure the user can choose the temp to test
</commit_message>
<xml_diff>
--- a/LWDM_Tx_4x25/LWDM 4x25 TEST PLAN.xlsx
+++ b/LWDM_Tx_4x25/LWDM 4x25 TEST PLAN.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DDisk\OSA Test\OSA Test Softwares\LWDM_Tx_4x25\LWDM_Tx_4x25\bin\Debug\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DDisk\OSA 测试项目\LWDM 4x25 Tx\LWDM_Tx_4x25_Code\LWDM_Tx_4x25\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
   <si>
     <t>intial all the euipment</t>
   </si>
@@ -48,10 +48,6 @@
   </si>
   <si>
     <t>Set the N1092A</t>
-  </si>
-  <si>
-    <t>false表示测试结果fail后，不继续后面的温度测试</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>TempSpan</t>
@@ -191,6 +187,25 @@
   </si>
   <si>
     <t>CH4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上个温度fail后，继续测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选中温度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弃用</t>
+  </si>
+  <si>
+    <t>弃用</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -289,30 +304,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -338,7 +333,33 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -352,18 +373,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -376,10 +392,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -690,14 +732,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.875" customWidth="1"/>
     <col min="4" max="4" width="20.125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.375" customWidth="1"/>
     <col min="14" max="14" width="26.25" customWidth="1"/>
@@ -713,438 +756,500 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="4"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="21"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="14" t="s">
         <v>4</v>
       </c>
+      <c r="D3" s="22"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="6">
         <v>25.78125</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="D5" s="22"/>
+    </row>
+    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="13">
+      <c r="B6" s="8">
         <v>0.125</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="22"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="9">
+        <v>20</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="22"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="14">
-        <v>20</v>
-      </c>
-      <c r="C9" s="9"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="B10" s="9">
+        <v>2.4</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="22"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="14">
-        <v>2.4</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="15">
+      <c r="B11" s="10">
         <v>0.2</v>
       </c>
-      <c r="C11" s="10"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="22"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="22"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="22"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="9">
         <v>21</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="C14" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="22"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="9">
+        <v>3.3</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="22"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="22"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="22"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B18" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C18" s="14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="D18" s="22"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="9">
+        <v>22</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="22"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="14">
-        <v>21</v>
-      </c>
-      <c r="C14" s="9"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="B20" s="9">
+        <v>3.3</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="22"/>
+    </row>
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="14">
-        <v>3.3</v>
-      </c>
-      <c r="C15" s="9" t="s">
+      <c r="B21" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="22"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="22"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="22"/>
+    </row>
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="9">
         <v>23</v>
       </c>
-      <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="C24" s="15"/>
+      <c r="D24" s="22"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="22"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="22"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="9">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="14">
-        <v>22</v>
-      </c>
-      <c r="C19" s="9"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="14">
-        <v>3.3</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="14">
-        <v>23</v>
-      </c>
-      <c r="C24" s="9"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="4"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="14">
-        <v>22</v>
-      </c>
-      <c r="C27" s="9"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="C27" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="22"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="C28" s="15"/>
+      <c r="D28" s="22"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="9"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+      <c r="C29" s="15"/>
+      <c r="D29" s="22"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B30" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="9"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
+      <c r="C30" s="15"/>
+      <c r="D30" s="22"/>
+    </row>
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B31" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="9"/>
-    </row>
-    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="9"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C31" s="15"/>
+      <c r="D31" s="22"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="12"/>
-      <c r="C32" s="4"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+      <c r="B32" s="7"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="22"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="22"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="22"/>
+    </row>
+    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="22"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="24"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="9">
+        <v>25</v>
+      </c>
+      <c r="C38" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="9">
+        <v>0</v>
+      </c>
+      <c r="C39" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="9">
+        <v>78</v>
+      </c>
+      <c r="C40" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="22"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="9">
+        <v>120</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="22"/>
+    </row>
+    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="10">
+        <v>300</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="23"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="7"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="22"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34" s="6"/>
-    </row>
-    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="C35" s="6"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" s="12"/>
-      <c r="C36" s="4"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" s="14">
-        <v>25</v>
-      </c>
-      <c r="C38" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B39" s="14">
-        <v>0</v>
-      </c>
-      <c r="C39" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B40" s="14">
-        <v>78</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="5" t="s">
+      <c r="D45" s="22"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B41" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="C41" s="6"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="5" t="s">
+      <c r="B46" s="9">
+        <v>60</v>
+      </c>
+      <c r="C46" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="14">
-        <v>120</v>
-      </c>
-      <c r="C42" s="6" t="s">
+      <c r="D46" s="22"/>
+    </row>
+    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B43" s="15">
+      <c r="B47" s="10">
         <v>300</v>
       </c>
-      <c r="C43" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B44" s="12"/>
-      <c r="C44" s="4"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
+      <c r="C47" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B46" s="14">
-        <v>60</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B47" s="15">
-        <v>300</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>11</v>
-      </c>
+      <c r="D47" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Modify Test Plan parameters' location
</commit_message>
<xml_diff>
--- a/LWDM_Tx_4x25/LWDM 4x25 TEST PLAN.xlsx
+++ b/LWDM_Tx_4x25/LWDM 4x25 TEST PLAN.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="65">
   <si>
     <t>intial all the euipment</t>
   </si>
@@ -74,10 +74,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>31，NRZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Clock</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -86,10 +82,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>GPIB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Vcc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -122,14 +114,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Mask</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100G LR</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Set TEC Out</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -146,10 +130,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Keithley 2000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Keithley 7001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -202,11 +182,100 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>弃用</t>
-  </si>
-  <si>
-    <t>弃用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Channel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1A</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BandWidth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AOP Offset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TempSpan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TimeOut</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>TempOffset</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>℃</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set AQ6730</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>StartWave_CH1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dBm</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>StopWave_CH1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>StartWave_CH2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>StartWave_CH3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>StartWave_CH4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>StopWave_CH4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StopWave_CH3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>StoptWave_CH2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set PM212</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power_Offse_CH1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power_Offse_CH2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power_Offse_CH3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power_Offse_CH4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -730,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O47"/>
+  <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -788,8 +857,8 @@
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>14</v>
+      <c r="B5" s="6">
+        <v>31</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>13</v>
@@ -798,7 +867,7 @@
     </row>
     <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="8">
         <v>0.125</v>
@@ -808,7 +877,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="13"/>
@@ -828,183 +897,177 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="9">
+        <v>2.4</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="22"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="9">
-        <v>20</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="22"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="B10" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="22"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="9">
-        <v>2.4</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="22"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="C11" s="16"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="22"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="13"/>
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>4</v>
+      </c>
       <c r="D12" s="22"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="9">
+        <v>3.3</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="22"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="22"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="22"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B16" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C16" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="22"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="D16" s="22"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="9">
+        <v>3.3</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="22"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="9">
-        <v>21</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="22"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="9">
-        <v>3.3</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="22"/>
-      <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="10">
-        <v>0.3</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="22"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="B18" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="C18" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="22"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>4</v>
-      </c>
       <c r="D18" s="22"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="9">
-        <v>22</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>46</v>
-      </c>
+      <c r="A19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="13"/>
       <c r="D19" s="22"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="9">
-        <v>3.3</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>24</v>
+        <v>2</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>4</v>
       </c>
       <c r="D20" s="22"/>
     </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>25</v>
-      </c>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="15"/>
       <c r="D21" s="22"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="13"/>
+      <c r="C22" s="15"/>
       <c r="D22" s="22"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>4</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C23" s="15"/>
       <c r="D23" s="22"/>
     </row>
     <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="9">
-        <v>23</v>
+        <v>37</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="22"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="13"/>
@@ -1014,168 +1077,176 @@
       <c r="A26" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="D26" s="22"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="9">
-        <v>22</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>47</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="14"/>
       <c r="D27" s="22"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="15"/>
+        <v>43</v>
+      </c>
+      <c r="B28" s="6">
+        <v>13.3</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="D28" s="22"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="22"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="24"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="22"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="22"/>
-    </row>
-    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="22"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="22"/>
+      <c r="A32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="9">
+        <v>25</v>
+      </c>
+      <c r="C32" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" s="25" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D33" s="22"/>
+        <v>26</v>
+      </c>
+      <c r="B33" s="9">
+        <v>0</v>
+      </c>
+      <c r="C33" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" s="25" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="22"/>
-    </row>
-    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
+      <c r="B34" s="9">
+        <v>78</v>
+      </c>
+      <c r="C34" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="9">
+        <v>0.5</v>
+      </c>
       <c r="C35" s="14"/>
       <c r="D35" s="22"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="24"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" s="25" t="s">
-        <v>45</v>
-      </c>
+      <c r="A36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="9">
+        <v>15</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="22"/>
+    </row>
+    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="10">
+        <v>300</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="23"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="9">
-        <v>25</v>
-      </c>
-      <c r="C38" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="D38" s="25" t="b">
-        <v>1</v>
-      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="21"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B39" s="9">
-        <v>0</v>
-      </c>
-      <c r="C39" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D39" s="25" t="b">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="22"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B40" s="9">
-        <v>78</v>
-      </c>
-      <c r="C40" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D40" s="25" t="b">
-        <v>1</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="22"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
-        <v>8</v>
+      <c r="A41" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="B41" s="9">
         <v>0.5</v>
@@ -1184,11 +1255,11 @@
       <c r="D41" s="22"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>9</v>
+      <c r="A42" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="B42" s="9">
-        <v>120</v>
+        <v>300</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>10</v>
@@ -1197,23 +1268,23 @@
     </row>
     <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="B43" s="10">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="D43" s="23"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B44" s="7"/>
       <c r="C44" s="13"/>
-      <c r="D44" s="22"/>
+      <c r="D44" s="21"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
@@ -1229,27 +1300,137 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B46" s="9">
+        <v>51</v>
+      </c>
+      <c r="B46" s="9"/>
+      <c r="C46" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" s="22"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="9"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="22"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" s="9"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="22"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49" s="9"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="22"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="9"/>
+      <c r="C50" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" s="22"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="9"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="22"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="9"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="22"/>
+    </row>
+    <row r="53" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53" s="10"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="23"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="B54" s="7"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="21"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" s="22"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" s="9">
+        <v>0</v>
+      </c>
+      <c r="C56" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D46" s="22"/>
-    </row>
-    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B47" s="10">
-        <v>300</v>
-      </c>
-      <c r="C47" s="20" t="s">
+      <c r="D56" s="22"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="9">
+        <v>0</v>
+      </c>
+      <c r="C57" s="14"/>
+      <c r="D57" s="22"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" s="9">
+        <v>0</v>
+      </c>
+      <c r="C58" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D47" s="23"/>
+      <c r="D58" s="22"/>
+    </row>
+    <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" s="9">
+        <v>0</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D59" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>